<commit_message>
Update kitchen and countries notebook
</commit_message>
<xml_diff>
--- a/Kitchen Remodel Quotes/Kitchen Counter Quotes.xlsx
+++ b/Kitchen Remodel Quotes/Kitchen Counter Quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sasoffice365-my.sharepoint.com/personal/peter_styliadis_sas_com/Documents/github repos/Data Projects/Kitchen Remodel Quotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{07C29E6C-B421-405F-8563-D7D23F3CCE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17AEDE77-DD7C-4832-AF49-0638A98DF6CF}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{07C29E6C-B421-405F-8563-D7D23F3CCE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2DB4773-A21F-4B65-BFFF-5555AAA63CBD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E67B438-0B4E-47CB-9780-A623E3DAFA56}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{1E67B438-0B4E-47CB-9780-A623E3DAFA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +460,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +468,7 @@
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -702,13 +704,13 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>2961</v>
+        <v>3358.62</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -721,14 +723,14 @@
       <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
-        <v>3431</v>
+      <c r="D13" s="2">
+        <v>3843.97</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,13 +744,13 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>3760</v>
+        <v>4188.6000000000004</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>